<commit_message>
res: corrige la matriz de sensibilidad
el centro (4,4) es la razón actual de solvencia
</commit_message>
<xml_diff>
--- a/res/matriz_sens.xlsx
+++ b/res/matriz_sens.xlsx
@@ -414,19 +414,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.339089998724946</v>
+        <v>1.348535280068247</v>
       </c>
       <c r="C3">
-        <v>2.041638947421406</v>
+        <v>2.280027247411239</v>
       </c>
       <c r="D3">
-        <v>2.92656854957775</v>
+        <v>3.618982841204426</v>
       </c>
       <c r="E3">
-        <v>3.981994865573362</v>
+        <v>5.427926478372039</v>
       </c>
       <c r="F3">
-        <v>5.189389904848076</v>
+        <v>7.745174434347612</v>
       </c>
     </row>
     <row r="4">
@@ -434,19 +434,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.046971871450337</v>
+        <v>1.002720984225978</v>
       </c>
       <c r="C4">
-        <v>1.647376054473046</v>
+        <v>1.746133973763164</v>
       </c>
       <c r="D4">
-        <v>2.428123002071207</v>
+        <v>2.849455207820629</v>
       </c>
       <c r="E4">
-        <v>3.383522754303974</v>
+        <v>4.383495450832996</v>
       </c>
       <c r="F4">
-        <v>4.498342231264492</v>
+        <v>6.398574505914165</v>
       </c>
     </row>
     <row r="5">
@@ -454,19 +454,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.8065270508919874</v>
+        <v>0.7363758790605551</v>
       </c>
       <c r="C5">
-        <v>1.310885312772756</v>
+        <v>1.32073792052963</v>
       </c>
       <c r="D5">
-        <v>1.989611748963632</v>
+        <v>2.21689655653529</v>
       </c>
       <c r="E5">
-        <v>2.84413095285421</v>
+        <v>3.500746455980269</v>
       </c>
       <c r="F5">
-        <v>3.863919965501135</v>
+        <v>5.232592204231606</v>
       </c>
     </row>
     <row r="6">
@@ -474,19 +474,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.6122323686717984</v>
+        <v>0.534354214691467</v>
       </c>
       <c r="C6">
-        <v>1.028418240630865</v>
+        <v>0.9868075587613082</v>
       </c>
       <c r="D6">
-        <v>1.609194703399661</v>
+        <v>1.704160804274016</v>
       </c>
       <c r="E6">
-        <v>2.363418920871885</v>
+        <v>2.764096942459139</v>
       </c>
       <c r="F6">
-        <v>3.286471884832927</v>
+        <v>4.23429477656448</v>
       </c>
     </row>
     <row r="7">
@@ -494,19 +494,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.4581302343964494</v>
+        <v>0.3833978806917301</v>
       </c>
       <c r="C7">
-        <v>0.7953722494822227</v>
+        <v>0.7285524660266689</v>
       </c>
       <c r="D7">
-        <v>1.284128482441412</v>
+        <v>1.294433490935827</v>
       </c>
       <c r="E7">
-        <v>1.940321342968963</v>
+        <v>2.157425595591394</v>
       </c>
       <c r="F7">
-        <v>2.766019714268476</v>
+        <v>3.389634940376918</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: errores en labels
</commit_message>
<xml_diff>
--- a/res/matriz_sens.xlsx
+++ b/res/matriz_sens.xlsx
@@ -1,21 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e64e3084cf54c9d/Documentos/Semestre 7/Pensiones/Proyecto/res/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_8F68FDCE8F79A8D366075C52F36E92F634188BAF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B271FC3-4589-49F8-B290-F21776A23878}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Inf</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +105,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +157,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +191,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +226,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,91 +402,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Inf</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>V1</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>V2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>V3</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>V4</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>V5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>5.793611978731801</v>
+        <f>C2-2</f>
+        <v>3.7936119787318008</v>
       </c>
       <c r="C2">
-        <v>7.793611978731802</v>
+        <v>5.7936119787318008</v>
       </c>
       <c r="D2">
-        <v>9.793611978731802</v>
+        <v>7.7936119787318017</v>
       </c>
       <c r="E2">
+        <v>9.7936119787318017</v>
+      </c>
+      <c r="F2">
         <v>11.7936119787318</v>
       </c>
-      <c r="F2">
-        <v>13.7936119787318</v>
-      </c>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>1.348535280068247</v>
+        <v>1.3485352800682471</v>
       </c>
       <c r="C3">
-        <v>2.280027247411239</v>
+        <v>2.2800272474112391</v>
       </c>
       <c r="D3">
         <v>3.618982841204426</v>
       </c>
       <c r="E3">
-        <v>5.427926478372039</v>
+        <v>5.4279264783720391</v>
       </c>
       <c r="F3">
-        <v>7.745174434347612</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>7.7451744343476117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1.002720984225978</v>
+        <v>1.0027209842259781</v>
       </c>
       <c r="C4">
         <v>1.746133973763164</v>
@@ -443,58 +483,58 @@
         <v>2.849455207820629</v>
       </c>
       <c r="E4">
-        <v>4.383495450832996</v>
+        <v>4.3834954508329957</v>
       </c>
       <c r="F4">
-        <v>6.398574505914165</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>6.3985745059141648</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>0.7363758790605551</v>
+        <v>0.73637587906055513</v>
       </c>
       <c r="C5">
-        <v>1.32073792052963</v>
+        <v>1.3207379205296299</v>
       </c>
       <c r="D5">
-        <v>2.21689655653529</v>
+        <v>2.2168965565352901</v>
       </c>
       <c r="E5">
         <v>3.500746455980269</v>
       </c>
       <c r="F5">
-        <v>5.232592204231606</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5.2325922042316062</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>0.534354214691467</v>
+        <v>0.53435421469146704</v>
       </c>
       <c r="C6">
-        <v>0.9868075587613082</v>
+        <v>0.98680755876130821</v>
       </c>
       <c r="D6">
         <v>1.704160804274016</v>
       </c>
       <c r="E6">
-        <v>2.764096942459139</v>
+        <v>2.7640969424591391</v>
       </c>
       <c r="F6">
-        <v>4.23429477656448</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>4.2342947765644796</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>0.3833978806917301</v>
+        <v>0.38339788069173009</v>
       </c>
       <c r="C7">
         <v>0.7285524660266689</v>
@@ -503,10 +543,10 @@
         <v>1.294433490935827</v>
       </c>
       <c r="E7">
-        <v>2.157425595591394</v>
+        <v>2.1574255955913939</v>
       </c>
       <c r="F7">
-        <v>3.389634940376918</v>
+        <v>3.3896349403769181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>